<commit_message>
Properly loading ABR hooks. Hook reactions rightfully export hook data in dictionaries.
</commit_message>
<xml_diff>
--- a/examples/new_abr/Shared model arrows.xlsx
+++ b/examples/new_abr/Shared model arrows.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="287">
   <si>
     <t>Name</t>
   </si>
@@ -785,9 +785,6 @@
   </si>
   <si>
     <t>relative discharge rate given high carriage of DR</t>
-  </si>
-  <si>
-    <t>p_admitted_infection</t>
   </si>
   <si>
     <t>probability a new admit is infected</t>
@@ -10977,10 +10974,10 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>239</v>
       </c>
       <c r="D12" s="5">
         <v>0.0</v>
@@ -10989,10 +10986,10 @@
     </row>
     <row r="13">
       <c r="A13" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>241</v>
       </c>
       <c r="D13" s="8">
         <v>0.0</v>
@@ -11000,10 +10997,10 @@
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>243</v>
       </c>
       <c r="D14" s="5">
         <v>0.1</v>
@@ -11011,10 +11008,10 @@
     </row>
     <row r="15">
       <c r="A15" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>244</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>245</v>
       </c>
       <c r="D15" s="8">
         <v>0.1</v>
@@ -11022,10 +11019,10 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>246</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>247</v>
       </c>
       <c r="D16" s="5">
         <v>0.2</v>
@@ -11036,10 +11033,10 @@
         <v>101</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>248</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>249</v>
       </c>
       <c r="D17" s="8">
         <v>0.125</v>
@@ -11050,10 +11047,10 @@
         <v>99</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D18" s="5">
         <v>0.25</v>
@@ -11064,7 +11061,7 @@
         <v>104</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D19" s="8">
         <v>0.8</v>
@@ -11075,10 +11072,10 @@
         <v>106</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D20" s="5">
-        <v>0.125</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="21">
@@ -11086,13 +11083,13 @@
         <v>108</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>254</v>
-      </c>
       <c r="D21" s="8">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="22">
@@ -11100,7 +11097,7 @@
         <v>125</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D22" s="5">
         <v>1.0</v>
@@ -11111,10 +11108,10 @@
         <v>155</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C23" s="40" t="s">
         <v>256</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>257</v>
       </c>
       <c r="D23" s="8">
         <v>0.2</v>
@@ -11125,7 +11122,7 @@
         <v>128</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D24" s="5">
         <v>0.0</v>
@@ -11136,7 +11133,7 @@
         <v>151</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C25" s="40"/>
       <c r="D25" s="8">
@@ -11148,7 +11145,7 @@
         <v>134</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D26" s="5">
         <v>3.0</v>
@@ -11156,13 +11153,13 @@
     </row>
     <row r="27">
       <c r="A27" s="37" t="s">
+        <v>260</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="8" t="s">
         <v>262</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>263</v>
       </c>
       <c r="D27" s="8">
         <v>2.0</v>
@@ -11173,7 +11170,7 @@
         <v>141</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D28" s="5">
         <v>0.1</v>
@@ -11184,7 +11181,7 @@
         <v>147</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D29" s="8">
         <v>0.05</v>
@@ -11195,7 +11192,7 @@
         <v>149</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D30" s="5">
         <v>0.05</v>
@@ -11206,7 +11203,7 @@
         <v>158</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D31" s="8">
         <v>0.01</v>
@@ -11214,10 +11211,10 @@
     </row>
     <row r="32">
       <c r="A32" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>269</v>
       </c>
       <c r="D32" s="5">
         <v>0.2</v>
@@ -11228,7 +11225,7 @@
         <v>7</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C33" s="43"/>
       <c r="D33" s="42">
@@ -11241,7 +11238,7 @@
         <v>163</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C34" s="47"/>
       <c r="D34" s="46">
@@ -11251,10 +11248,10 @@
     </row>
     <row r="35">
       <c r="A35" s="41" t="s">
+        <v>271</v>
+      </c>
+      <c r="B35" s="42" t="s">
         <v>272</v>
-      </c>
-      <c r="B35" s="42" t="s">
-        <v>273</v>
       </c>
       <c r="C35" s="43"/>
       <c r="D35" s="42">
@@ -11264,10 +11261,10 @@
     </row>
     <row r="36">
       <c r="A36" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="B36" s="46" t="s">
         <v>274</v>
-      </c>
-      <c r="B36" s="46" t="s">
-        <v>275</v>
       </c>
       <c r="C36" s="47"/>
       <c r="D36" s="46">
@@ -11277,13 +11274,13 @@
     </row>
     <row r="37">
       <c r="A37" s="41" t="s">
+        <v>275</v>
+      </c>
+      <c r="B37" s="42" t="s">
         <v>276</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="C37" s="42" t="s">
         <v>277</v>
-      </c>
-      <c r="C37" s="42" t="s">
-        <v>278</v>
       </c>
       <c r="D37" s="42">
         <v>0.05</v>
@@ -11292,10 +11289,10 @@
     </row>
     <row r="38">
       <c r="A38" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="B38" s="46" t="s">
         <v>279</v>
-      </c>
-      <c r="B38" s="46" t="s">
-        <v>280</v>
       </c>
       <c r="C38" s="47"/>
       <c r="D38" s="46">
@@ -11305,10 +11302,10 @@
     </row>
     <row r="39">
       <c r="A39" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="B39" s="42" t="s">
         <v>281</v>
-      </c>
-      <c r="B39" s="42" t="s">
-        <v>282</v>
       </c>
       <c r="C39" s="43"/>
       <c r="D39" s="42">
@@ -11318,13 +11315,13 @@
     </row>
     <row r="40">
       <c r="A40" s="49" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40" s="50" t="s">
         <v>283</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="C40" s="50" t="s">
         <v>284</v>
-      </c>
-      <c r="C40" s="50" t="s">
-        <v>285</v>
       </c>
       <c r="D40" s="50">
         <v>0.05</v>
@@ -11351,10 +11348,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>286</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="2">

</xml_diff>